<commit_message>
latest changes regarding profile
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/ProjectPulse.xlsx
+++ b/src/test/resources/testData/ProjectPulse.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -42,16 +42,135 @@
   </si>
   <si>
     <t>12345</t>
+  </si>
+  <si>
+    <t>TC_002</t>
+  </si>
+  <si>
+    <t>clientName</t>
+  </si>
+  <si>
+    <t>czTest</t>
+  </si>
+  <si>
+    <t>clientNotes</t>
+  </si>
+  <si>
+    <t>physicalAddress1</t>
+  </si>
+  <si>
+    <t>physicalAddress2</t>
+  </si>
+  <si>
+    <t>physicalState</t>
+  </si>
+  <si>
+    <t>physicalCity</t>
+  </si>
+  <si>
+    <t>physicalZip</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>billingAddress1</t>
+  </si>
+  <si>
+    <t>billingAddress2</t>
+  </si>
+  <si>
+    <t>billingCountry</t>
+  </si>
+  <si>
+    <t>billingState</t>
+  </si>
+  <si>
+    <t>billingCity</t>
+  </si>
+  <si>
+    <t>billingZip</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>czNotes</t>
+  </si>
+  <si>
+    <t>czBanglore</t>
+  </si>
+  <si>
+    <t>czBanglore2</t>
+  </si>
+  <si>
+    <t>Tamilnadu</t>
+  </si>
+  <si>
+    <t>chennai</t>
+  </si>
+  <si>
+    <t>billingCz</t>
+  </si>
+  <si>
+    <t>billingcz</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>600078</t>
+  </si>
+  <si>
+    <t>Chennai</t>
+  </si>
+  <si>
+    <t>Ms.</t>
+  </si>
+  <si>
+    <t>Gautham</t>
+  </si>
+  <si>
+    <t>Muru</t>
+  </si>
+  <si>
+    <t>gau@gamil.com</t>
+  </si>
+  <si>
+    <t>9600363826</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -74,14 +193,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -360,19 +482,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -382,8 +516,68 @@
       <c r="C1" t="s">
         <v>3</v>
       </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -394,8 +588,82 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" t="s">
+        <v>34</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" t="s">
+        <v>38</v>
+      </c>
+      <c r="S3" t="s">
+        <v>39</v>
+      </c>
+      <c r="T3" t="s">
+        <v>40</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="V3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
profile End TO end
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/ProjectPulse.xlsx
+++ b/src/test/resources/testData/ProjectPulse.xlsx
@@ -155,7 +155,7 @@
     <t>TC_003</t>
   </si>
   <si>
-    <t>czTest7</t>
+    <t>czTestgau95</t>
   </si>
 </sst>
 </file>
@@ -488,7 +488,7 @@
   <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>